<commit_message>
Atualização da logo laranja + Planilha completa
</commit_message>
<xml_diff>
--- a/iniciativas.xlsx
+++ b/iniciativas.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Recursos Humanos\PROJETOS RH\Projetos_2025\Cultura e Clima\VALORES QUE MOVEM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ABE5A34-87C4-463E-9776-46CE219E37D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE0D296E-64AE-4347-BFB5-A73C0400C630}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="148">
   <si>
     <t xml:space="preserve">Nome colaborador(a)
 </t>
@@ -38,19 +38,75 @@
 </t>
   </si>
   <si>
+    <t>Ana Flávia Trevisan Ieno</t>
+  </si>
+  <si>
     <t>Matriz</t>
   </si>
   <si>
     <t>Pedro Henrique Almeida Lima</t>
   </si>
   <si>
+    <t>Fernando Tryferis</t>
+  </si>
+  <si>
+    <t>Biza/ Serv</t>
+  </si>
+  <si>
     <t>Igor Daniel Ruiz</t>
   </si>
   <si>
     <t xml:space="preserve">Joice Agnes Pereira Gomes </t>
   </si>
   <si>
+    <t>Rosa Virginia Bassi Sivieiro</t>
+  </si>
+  <si>
+    <t>Marcelo Augusto de Campos Araujo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Desenvolvimento da EVA (Enhanced Virtual Assistant), uma solução baseada em Inteligência Artificial (IA) criada para auxiliar todas as áreas na construção e padronização de Instruções de Trabalho (ITs).
+A iniciativa busca garantir agilidade, consistência e alinhamento ao modelo corporativo, permitindo que a IA aprenda com as ITs já publicadas pelo Escritório de Processos e passe a gerar automaticamente novas instruções, mantendo o mesmo padrão estrutural, de linguagem e formatação adotado pela empresa.
+</t>
+  </si>
+  <si>
     <t xml:space="preserve">Vitoria Ferreira Dos Santos </t>
+  </si>
+  <si>
+    <t>ADRIANE LISBOA DANTAS</t>
+  </si>
+  <si>
+    <t>FLAVIA BRAGA SILVEIRA</t>
+  </si>
+  <si>
+    <t>SIMONE SANTOS DE GREGORIO</t>
+  </si>
+  <si>
+    <t>VICTORIA VIANA BATISTA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marcelo Bezerra </t>
+  </si>
+  <si>
+    <t>HF100</t>
+  </si>
+  <si>
+    <t>William Mendes de Paula</t>
+  </si>
+  <si>
+    <t>Caio Scandiuzzi Valente Coimbra</t>
+  </si>
+  <si>
+    <t>Jaqueline Souza Silva</t>
+  </si>
+  <si>
+    <t>Kleber Araujo de Moraes</t>
+  </si>
+  <si>
+    <t>José Sérgio</t>
+  </si>
+  <si>
+    <t>Matheus Pereira Rosa</t>
   </si>
   <si>
     <t>Priscila Rosa Barcia</t>
@@ -70,15 +126,132 @@
 • Elaborou uma base inteligente para ao final de cada instalação, o time técnico informar se faltou ou sobrou material e assim otimizar nossos kit's para maior assertividade e atualização dos projetos. </t>
   </si>
   <si>
+    <t>Osvaldo Aparecido Machado</t>
+  </si>
+  <si>
+    <t>Alex Rodrigues de Morais</t>
+  </si>
+  <si>
+    <t>Pamela de Moraes Ezequiel</t>
+  </si>
+  <si>
+    <t>Daniela Vieira Lima</t>
+  </si>
+  <si>
+    <t>Maria  das Neves Fernandes</t>
+  </si>
+  <si>
+    <t>Claudonir Correia Gomes</t>
+  </si>
+  <si>
+    <t>Antonio Ryvaldo Ferreira Neris</t>
+  </si>
+  <si>
+    <t>GHT Parauapebas</t>
+  </si>
+  <si>
+    <t>Lucas Alves de Carvalho</t>
+  </si>
+  <si>
+    <t>Gian Morelli</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FABRICIO DO SANTOS RIBEIRO </t>
+  </si>
+  <si>
+    <t>GHT Belém</t>
+  </si>
+  <si>
     <t xml:space="preserve">Bruna Toledo Veitonis Nham </t>
   </si>
   <si>
+    <t>DIOGO ROSA</t>
+  </si>
+  <si>
+    <t>Elias Souza Santos Junior</t>
+  </si>
+  <si>
+    <t>GHT Serviços</t>
+  </si>
+  <si>
+    <t>MARIA LOUIZE IVANA FONSECA DA SILVA</t>
+  </si>
+  <si>
+    <t>Priscilla Dafne Carvalho Vaz</t>
+  </si>
+  <si>
+    <t>GHT Contagem</t>
+  </si>
+  <si>
     <t>Carlos Eduardo Merigo</t>
   </si>
   <si>
+    <t>Gabriel da Silva Gopfert Pinto</t>
+  </si>
+  <si>
+    <t>Gabriel Gava, Bernardo Sousa, André Bezerra, Cleiton Hora e Reginaldo Santos</t>
+  </si>
+  <si>
+    <t>Juliana Cipriano Nery</t>
+  </si>
+  <si>
+    <t>Daisy Plastina de Barros</t>
+  </si>
+  <si>
+    <t>Juliana Santos Araujo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kelvin Barbosa da Silva </t>
+  </si>
+  <si>
+    <t>Mariana Pereira</t>
+  </si>
+  <si>
+    <t>Larissa Lima da Costa</t>
+  </si>
+  <si>
+    <t>Renata de Freitas Silva</t>
+  </si>
+  <si>
+    <t>Kaoma Rodrigues da Silva</t>
+  </si>
+  <si>
+    <t>Natalia De Jesus Franca</t>
+  </si>
+  <si>
+    <t>Daniele de Oliveira Albuquerque</t>
+  </si>
+  <si>
+    <t>Foi implementada em 2025 uma melhoria no processo de pagamento via arquivo, por meio da adoção de uma rotina sistemática de varredura no DDA (Débito Direto Autorizado), com foco na identificação antecipada de títulos em vias de protesto antes do vencimento. Essa conferência preventiva passou a fazer parte da rotina diária de Contas a Pagar, permitindo identificar inconsistências, divergências de registro ou pendências com fornecedores em tempo hábil para tratamento. Dessa forma, ao identificar um título em iminência de protesto, antes que ocorra a negativação do CNPJ, é acionado o time responsável para providenciar o lançamento da nota fiscal vinculada ao título em questão e regularizar a situação dentro do prazo.</t>
+  </si>
+  <si>
+    <t>Daniele Meireles</t>
+  </si>
+  <si>
+    <t>Vanessa Feitosa dos Santos</t>
+  </si>
+  <si>
+    <t>Leticia Amelia Liberato</t>
+  </si>
+  <si>
+    <t>Foram implementadas melhorias na tela de recebimento de CT-e, permitindo pesquisa em lote, seleção múltipla e alterações massivas dos campos de vencimento, tipo de entrada e data de entrada. Essas funcionalidades foram desenvolvidas para agilizar ajustes necessários quando ocorrem anomalias no processo de CT-e que exigem intervenção manual em grande volume de documentos.</t>
+  </si>
+  <si>
+    <t>Rafael Paulino Bernardo</t>
+  </si>
+  <si>
+    <t>João Pedro Barbosa Bochi Nogueira</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Camilla Trovatti </t>
+  </si>
+  <si>
     <t>AREA</t>
   </si>
   <si>
+    <t>RH</t>
+  </si>
+  <si>
     <t>GRANDE PORTE</t>
   </si>
   <si>
@@ -91,7 +264,43 @@
     <t>CADASTROS</t>
   </si>
   <si>
+    <t>PLANEJAMENTO</t>
+  </si>
+  <si>
+    <t>FILIAIS</t>
+  </si>
+  <si>
+    <t>BIZA</t>
+  </si>
+  <si>
+    <t>PLANEJAMENTO ESTRATÉGICO</t>
+  </si>
+  <si>
+    <t>TI</t>
+  </si>
+  <si>
+    <t>SGI BIZA</t>
+  </si>
+  <si>
+    <t>TRIBUTÁRIO/ CONTABILIDADE</t>
+  </si>
+  <si>
+    <t>FINANCEIRO</t>
+  </si>
+  <si>
     <t>ADM. VENDAS</t>
+  </si>
+  <si>
+    <t>GHT SERVIÇOS</t>
+  </si>
+  <si>
+    <t>VAREJO</t>
+  </si>
+  <si>
+    <t>SMP PA</t>
+  </si>
+  <si>
+    <t>LOGÍSTICA</t>
   </si>
   <si>
     <t xml:space="preserve">
@@ -110,6 +319,50 @@
 A IA analisar os CNAEs de atuação do cliente; verifica se é ISS ou ICMS e devolve com a informação de contribuição tributária correta.</t>
   </si>
   <si>
+    <t xml:space="preserve">Apoio na elaboração de feedbacks:
+Utiliza a IA para estruturar feedbacks de forma mais clara, objetiva e alinhada aos comportamentos esperados, garantindo comunicação assertiva e coerente.
+Apoio na construção de PDIs:
+Organização dos objetivos, ações de desenvolvimento, tornando os PDIs mais estratégicos, personalizados e facilmente aplicáveis.
+Desenvolvimento de apresentações:
+IA cria roteiros, organiza conteúdo e torna apresentações mais didáticas e visuais, aumentando a clareza e a qualidade das entregas.
+Geração e estruturação de projetos:
+A IA ajuda na pesquisa, benchmarking, organização de etapas e definição de indicadores, acelerando a criação de projetos mais robustos e fundamentados.
+Análises estruturais para revisão de processos:
+IA apoia diagnósticos, mapeamentos e identificação de pontos críticos nos processos, contribuindo para entregas mais rápidas e eficazes.
+</t>
+  </si>
+  <si>
+    <t>Projeto de PLR – Remuneração: Todo o material do projeto conta com o apoio de IA. Um exemplo disso são as "pílulas" informativas que são enviadas quinzenalmente aos funcionários, abordando temas relacionados a benefícios e remuneração. Essas pílulas estão sendo criadas com o uso do NotebookLM, além das ferramentas Tess.
+Além disso, o material de treinamento sobre Remuneração foi personalizado, com a criação de imagens, adequando o conteúdo para os diferentes públicos da organização.</t>
+  </si>
+  <si>
+    <t>Utiliza a IA como apoio na criação de suas apresentações e relatórios, deixando os materiais mais atrativos e, até mesmo, interativos.</t>
+  </si>
+  <si>
+    <t>Ivan Hideki Kobayashi</t>
+  </si>
+  <si>
+    <t>Utiliza IA para formatar planilhas do sistema; tirar dúvidas trabalhistas relacionadas a área, dar respostas de e-mails corporativos com mais assertividade e edição/alteração de documentação. Essas ações trazem maior assertividade e otimização do tempo.</t>
+  </si>
+  <si>
+    <t>Usa a IA em busca de ser mais objetiva e assertiva em análise em planilha como assistência médica, respostas dos e-mails corporativos e montagem do PDI.</t>
+  </si>
+  <si>
+    <t>Usa a IA para responder de e-mails corporativos, onbter embasamentos trabalhistas e montar vídeos com Avatar para o setor esclarecendo dúvidas; como: Folha, férias, benefícios, pontos, admissão e SST.</t>
+  </si>
+  <si>
+    <t>Usa a IA para melhor montagem dos invites, tirar dúvidas relacionadas à legislação trabalhista e obter melhores respostas nos e-mails corporativos. Com o projeto valores que movem está desenvolvendo Agente de Políticas e Chatbot, buscando esclarecer dúvidas dos colaboradores de forma rápida e prática.</t>
+  </si>
+  <si>
+    <t>Tem se dedicado a testar algumas ferramentas de IA para otimizar a geração de código de programação. Desenvolveu uma integração com o novo sistema de pedidos do cliente, utilizando o python para adequar o código.</t>
+  </si>
+  <si>
+    <t>Tem se destacado pela utilização de IA para geração de códigos de programação e testado diversas ferramentas propostas. Utilização de IA para programação da nova versão da GHTIA Chat.</t>
+  </si>
+  <si>
+    <t>Tem se destacado no desenvolvimento de automações em phyton para coleta de dados. Um dos projetos é a automação diária para coleta informações de entrega para cálculos de OTIF para Gestão de Pedidos/Contratos.</t>
+  </si>
+  <si>
     <t>Google Ads: Com apoio da IA, o sistema analisa o relatório e pontos estratégicos, ressaltando performance e quais ajustes precisam ser feitos para melhorar os resultados.
 _x000B_Facebook Ads: Atuação com dois agentes de IA — um focado em Google Ads e outro em Facebook Ads. Nas campanhas mensais de Facebook, o agente faz uma leitura completa do cenário, identifica as melhores estratégias de investimento e estuda a região ideal para segmentação, trazendo dados sobre público, comportamento e concorrência local._x000B_
 Eventos corporativos e feiras: A IA apoia na criação checklists inteligentes com prazos para cada tarefa, acompanhar datas de pagamento, montagem e desmontagem de estandes, e analisa o perfil do público que vai visitar o evento._x000B_</t>
@@ -123,6 +376,276 @@
   </si>
   <si>
     <t>Padronizou um processo: squad multidisciplinar, indicadores alinhados e campanhas contínuas. Essa ação de acompanhamento do projeto de itens sem giro trouxe redução expressiva do estoque e engajamento de todas as áreas comerciais. Realizou uma proposta criativa com avatar (prompt) das "guardiãs das listas" (Gameflow).</t>
+  </si>
+  <si>
+    <t>Reutilização de materiais de insumo na filial. Ex.: Papelão/ fita de arquear/ plástico filme/ pallets e papel A4.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transformação Sistêmica do Fechamento Contábil — De Processo Manual para Automação Inteligente Replicável
+Através de benchmark com a solução desenvolvida pelo Claudonir (mesmo time),  o colaborador desenvolveu códigos VBA complementares que automatizam as atividades mais manuais e propensas a erros com a utilização do chat GPT, e demonstrou o verdadeiro espírito de inovação coletiva ao tornar essas soluções replicáveis para toda a equipe. Uma iniciativa que reduz significativamente o tempo de fechamento e eleva o padrão de excelência operacional de toda a área.
+Com isso resolveu uma sequência de problemas que afetam o fechamento contábil:
+Etapa 1 - Conciliação Contábil (Manual antes):
+Preparar bases de dados
+Identificar valores batidos
+Identificar estornos
+Apontar  e tratar diferenças
+Fazer isto conta a conta (extremamente demorado)
+Etapa 2 - Validação de Bases (Manual antes):
+Validar diferenças com relatório suporte (contas a pagar / contas a receber)
+Comparar múltiplas colunas
+Identificar títulos batidos
+Identificar divergências para análise
+O colaborador não criou uma ferramenta "para especialistas em VBA". A solução é tão simples que qualquer usuário pode usar:
+Selecionar arquivo contábil
+Executar VBA
+Receber resultado estruturado
+Analisar apenas as diferenças
+</t>
+  </si>
+  <si>
+    <t>Melhoria de Processo &gt; Redução de Custo Houve uma redução significativa dos custos de manutenção do centro de usinagem G020. Foi realizada a substituição do disco do trocador de ferramentas da máquina, uma vez que o componente original utilizava um suporte que apresentava quebras frequentes. Cada suporte tinha custo unitário de R$ 665,24, além de demandar um processo de manutenção complexo.
+A substituição foi feita por um disco compatível com um novo modelo de suporte, cujo valor é de R$ 55,99, representando uma redução de 91% em relação ao custo anterior. Além disso, o procedimento de manutenção para troca desse suporte tornou-se consideravelmente mais simples. (Conforme Projeto de Ideias Biza nº 140.)</t>
+  </si>
+  <si>
+    <t>Organização e alinhamento do portfólio de projetos da Diretoria Comercial.  
+Identifiquei no Project Model Canvas Constructor uma oportunidade de usar IA não só como ferramenta de automação, mas como um “facilitador virtual” de planejamento de projetos.
+Usei o Project Model de apoio para estruturar, de forma padronizada, o escopo dos projetos, seguindo a lógica do Project Model.
+Na prática, o uso aconteceu em três frentes principais:
+a) Estruturação guiada do escopo dos projetos comerciais
+Para cada projeto comercial, utilizei a IA para conduzir, passo a passo, as seções:
+POR QUÊ: Justificativa, Objetivo SMART e Benefícios
+O QUÊ: Produto/serviço e principais requisitos
+QUEM: Stakeholders externos e equipe envolvida
+COMO: Premissas, grupos de entregas, restrições
+QUANDO/QUANTO: Riscos, linha do tempo e custos estimados
+A IA fazia uma pergunta de cada vez, o que me ajudava a organizar o raciocínio e transformar ideias dispersas em um escopo claro, coerente e alinhado com a realidade do GHT.
+b) Transformação em canvas visual padronizado
+Após a coleta das informações de cada projeto, o Project Model organizava tudo em um layout visual da própria plataforma, pronto para ser compartilhado com os responsáveis das áreas. Isso passou a ser usado como “peça oficial” de escopo: em vez de textos soltos ou e-mails longos, cada projeto comercial passou a ter um Project Model Canvas como referência única.
+c) Apoio à priorização e comunicação com as áreas internas
+Com os projetos comerciais descritos em um formato padrão, ficou muito mais fácil comparar iniciativas quanto a: alinhamento estratégico, benefícios esperados, riscos, esforço e custo.</t>
+  </si>
+  <si>
+    <t>Aplicação do formato de BI nas apresentações e tratamento da carteira de pedidos geradas pelo planejador de estoque do complexo de Carajás.</t>
+  </si>
+  <si>
+    <t>Criou Agente: Com o objetivo de melhorar o acompanhamento das demandas das filiais e tornar o fluxo de trabalho mais organizado, a Camilla desenvolveu um agente específico para apoiar esse controle. Esse Agente passou a atuar como um facilitador da rotina, auxiliando no monitoramento de entregas, prazos e pendências.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Automação Inteligente de Conciliações Bancárias e de Faturamento — Transformando Processos Manuais em Soluções Escaláveis com IA
+O colaborador identificou que dois processos críticos de conciliação contábil — banco e faturamento — consumiam tempo significativo em atividades repetitivas e propensas a erros. Buscou benchmarking para entender uma aplicação utilizada no ambiente da tesouraria, utilizou IA (ChatGPT) para desenvolver código VBA que transformaram conciliações manuais em processos inteligentes, automáticos e confiáveis. Uma iniciativa que exemplifica como a IA pode ser uma aliada estratégica da contabilidade moderna.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Desenvolvemos uma integração automática entre o SPR e o CRM, contemplando a criação e qualquer alteração realizada nos grupos econômicos.
+A integração automatizada de dados entre sistemas, permitiu a transferência eficiente e, em tempo real, de informações de um grupo de clientes para outro sistema corporativo, garantindo equidade das informações financeiras. Esta automação eliminou processos manuais e duplicados anteriormente necessários, reduzindo significativamente o tempo de processamento e minimizando riscos de erros humanos na manipulação de dados. A solução garante maior consistência e confiabilidade na sincronização das informações entre as plataformas, otimizando o fluxo de trabalho e contribuindo para a melhoria da eficiência operacional da organização, além de garantir integridade das informações entre um sistema e outro, pois a origem ficou concentrada no SPR.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A melhoria implementada consistiu na criação da funcionalidade “Replicar CFOP” na tela de edição dos itens da Nota Fiscal. A partir da identificação da necessidade de otimizar o processo de classificação fiscal, a colaboradora analisou o fluxo atual, mapeou o retrabalho existente na edição item a item e propôs a automatização da replicação do CFOP.
+A partir dessa proposta, a equipe de TI desenvolveu a opção disponível por meio do clique com o botão direito na coluna CFOP, permitindo que o usuário copie o CFOP de um item e aplique automaticamente aos demais da nota. A solução torna o processo mais ágil, padronizado e reduz a possibilidade de erros operacionais.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O projeto consistiu na automatização completa da alteração de situação de títulos por meio da leitura do arquivo de retorno bancário. O processo demandava no mínimo 1 hora diária de trabalho, além do alto risco de falhas operacionais, retrabalho e inconsistências de dados.
+O que foi transformado com a automação:
+O fluxo passou a ser 100% automático, a partir da simples leitura do arquivo de retorno bancário. O sistema agora:
+• Atualiza automaticamente o status dos títulos;
+• Bloqueia as fichas de forma imediata;
+• Replica o bloqueio automaticamente para clientes de grupo;
+• Registra automaticamente o histórico de títulos;
+• Permite o desbloqueio em lote e registro de pagamento de forma igualmente automática.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_x000B_• Idealização e estruturação do Programa de Ideias BIZA (melhoria contínua), desenvolvimento de catálogo de iniciativas (site).
+_x000B_• Desenvolvimento do Modelo Matemático de Sequenciamento de OF no SPRWEB, trazendo inteligência operacional e eliminando dependência de planilhas manuais (acompanhar PRODUÇÃO – o sistema define prioridade do item) – usando desde junho
+_x000B_• Automação inteligente no fluxo de reclamações do CQP, garantindo disparo automático de e-mails e maior confiabilidade nas tratativas (uso do power automate da Microsoft). Preenche planilha com 47 colunas e a cada 2h um e-mail é enviado, aos envolvidos CASO a planilha tenha alterações.
+_x000B_• Criação do Painel de Metas BIZA, reunindo metas salariais, faixas, N3, rotina e PLR em uma plataforma acessível e atualizado em tempo real para cálculo de faixas salariais. É um link (site) para que todos tenham acesso de forma mais rápida e prática.
+_x000B_• Criação e implantação do PORTAL Informações Gerais BIZA, unificando documentos, indicadores e links estratégicos em um único ambiente digital para acesso fácil de todos os colaboradores da BIZA (os links criados nas outras ferramentas estão aqui também).
+_x000B_• Padronização do fluxo de gestão de óleo no setor CNC, reduzindo desperdícios, riscos de transbordo e fortalecendo controles ambientais. 
+_x000B_• Apoio na implementação dos Dashboards automáticos no SIGO (power BI), com indicadores em tempo real e ganho de agilidade na gestão de ações e documentos.
+</t>
+  </si>
+  <si>
+    <t>Melhoria contínua - Iniciativas realizadas no GHT Serviços em 2025:
+Implantação de sistemas de gestão: KANBAN e Gantt diário
+Melhoria da infraestrutura, layout e organização da oficina
+Padronização e identificação operacional (registros)
+Modernização da ferramentaria e usinagem
+Reestruturação da área de peritagem e gestão de resíduos
+Inspeções estruturadas nos equipamentos de içamento
+Ativação do tanque de produto químico
+Aquisições para eficiência e segurança: mangueiras, cintas, lixadeiras
+Redução de custos e reaproveitamento interno</t>
+  </si>
+  <si>
+    <t>Com benchmarking com o Diogo, o colaborador realizou automações para o dia a dia, e melhorou processos substituindo relatórios digitais no lugar de papel, automatizando o envio de e-mails e construindo DASHBOARDS de algumas planilhas para melhor visualização de resultados e indicadores.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AGENTE MKP ESTRATÉGICO - Solução de IA para Proteção da Lucratividade
+Descrição da Solução
+O Agente MKP Estratégico é uma solução de inteligência artificial conversacional especializada em análise de dados de precificação e performance de vendas, desenvolvida especificamente para proteger e otimizar a lucratividade.
+Diferenciais Técnicos:
+•	Framework ROSES para estruturação de prompts estratégicos
+•	Análise Multidimensional: Gerências × Famílias × Temporal
+•	Recomendações Contextualizadas baseadas nas regras de negócio
+•	Memória Organizacional com conhecimento institucional 
+</t>
+  </si>
+  <si>
+    <t>Tivemos avanços significativos no projeto de organização do 204, incluindo a finalização do novo layout do Centro de Distribuição e o fortalecimento do projeto de produtividade. Essas entregas consolidam uma base mais estruturada para nossas operações, alinhando fluxo e processos. Com o apoio da IA, conseguimos evoluir os projetos em tempo recorde. Com isso ainda antecipamos alguns dados para o próximo ano do projeto Código Bom, que será um dos principais vetores de melhoria operacional. Esse conjunto de pilares irá direcionar e sustentar todas as iniciativas de melhoria e implantações setoriais, garantindo coerência entre as áreas e acelerando nossa capacidade de resposta.</t>
+  </si>
+  <si>
+    <t>Ferramenta de análise dedicada (EXCEL) – realiza a análise de itens com muita consulta mas sem estoque: a planilha mostra que pode ser um produto que podemos começar a comprar. A indicação dos produtos é enviada ao responsável para tomada de decisão:
+Identificação dos itens com consulta sem demanda no Planejamento de Estoque diário_x000B_Identificação dos itens com consulta com demanda sem compra no Planejamento de Estoque diário</t>
+  </si>
+  <si>
+    <t>Colaboradora usa IA no dia a dia para:
+• Identificação de peças com códigos parciais (P559… qual filtro Donaldson seria?); _x000B_• Fotos dos itens;_x000B_• Confirmação de compatibilidade entre máquina, modelo e número de série; _x000B_• Tradução de códigos (cotação por fotos enviadas pelos clientes varejo e contrato);_x000B_• E-mail – Solicito que ajuste conforme a mensagem que quero transmitir; _x000B_• Educação – Transformar arquivos de PDF em PODCAST, facilitando o estudo no trajeto até o trabalho;_x000B_• Planilhas dos BIDs, solicito a limpeza da lista conforme necessidade.</t>
+  </si>
+  <si>
+    <t>O João realizou a automatização da planilha de planejamento de estoque da área de Motores, trazendo mais rapidez e precisão para o acompanhamento dos itens. Ele também passou a utilizar recursos de IA para ganhar agilidade nas tarefas do dia a dia, como análise de planilhas, pesquisas de informações de fornecedores e peças, manipulação de arquivos e criação de textos. Além disso, desenvolveu um Agente de webscraping para itens de motores, que busca automaticamente as principais informações dos produtos em sites de concorrentes e fornecedores, facilitando a consulta e comparação dos dados.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Em 2025, foi desenvolvida e implementada a automatização da contabilização dos pagamentos das guias, integrando o sistema SPR ao ERP Sispro. O principal objetivo da iniciativa foi eliminar os lançamentos manuais realizados pela Tesouraria, promovendo mais eficiência, padronização e confiabilidade às informações financeiras da companhia.
+A solução aprimorou a comunicação entre os sistemas, permitindo que as guias pagas por operação fossem automaticamente identificadas e contabilizadas conforme o banco de pagamento. Foram incorporados também mecanismos para o tratamento de exceções — como pagamentos manuais, ajustes e estornos, assegurando flexibilidade operacional e consistência dos dados.
+O projeto foi iniciativa do Contas a Pagar e desenvolvido de forma colaborativa com impacto nas áreas de Tesouraria, Contabilidade e Financeiro, consolidando o uso da tecnologia como aliada na otimização de processos, redução de atividades manuais e fortalecimento do controle contábil e fiscal.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Em 2025, foi implantado um novo processo de Recuperação de Crédito junto aos nossos fornecedores. A partir desse ano ficou estabelecido que os créditos gerados pelas devoluções de peças fossem recuperados no menor prazo possível e que tivesse uma gestão à vista e mais eficiente na recuperação desses créditos, seja com a devolução dos valores ou abatimento em títulos a pagar. Para isso, criamos um relatório de acompanhamento semanal. Neste novo processo, ficamos como área centralizadora da comunicação com o fornecedor e nossos times internos (Compras, Fiscal, Logística), gerando melhor interface e maior dinamismo na cobrança, seja interna ou externa. </t>
+  </si>
+  <si>
+    <t>Desenvolvimento do relatório de notas fiscais canceladas no Flow: Esse relatório foi a última etapa dos processos de automação e melhorias envolvendo o cancelamento das notas fiscais. Esse relatório chega por e-mail, além disso, também foi automatizado o processo de consulta e validação de NFs no sitema.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Em 2025, o colaborador desenvolveu e implementou um macrofluxo padronizado para separação, conferência e embarque, estruturando processos, criando KPIs de acurácia e desempenho, reorganizando embarques por peso e dimensão com plano-grama, aplicando Kanban para identificação de cargas, melhorando telas do SPR e atuando como ponto focal entre setores e filiais para garantir governança, previsibilidade e comunicação clara. 
+Além disso, consolidou ferramentas internas, aplicou metodologias Lean Six Sigma, criou métricas operacionais, otimizou rotinas, estruturou controles e aprimorou a gestão de estoque através de indicadores, melhorias sistêmicas e práticas que transformaram o ambiente em um processo orientado por dados e sustentado por fluxos mais eficientes e intuitivos.
+ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Dados Mais Limpos e Organizados!
+• Planilhas Sem Erro: A IA está cuidando de corrigir e formatar as planilhas do Excel automaticamente, deixando-as prontas para o nosso Sistema SPR (evitando longas digitações) .
+• "De-Para" com a ajuda da IA que traduz e converte códigos de produtos de outras empresas para os nossos códigos internos de forma automática. Cadastro e cotação, agora, são muito mais rápidos.
+2. Cotação: Velocidade Máxima
+• Transformando Imagem em Dados: Sabe aquelas fotos ou imagens de cotações? Estou usando uma IA  para extrair os dados delas e transformar em formato Excel e com comando Ctrl + I lanço no SPR. Isso acelera o retorno de resposta ao cliente.  
+3. Comunicação: E-mails formais 
+• Texto Profissional Sem Esforço: Uso ferramentas de IA para revisar e refinar meus e-mails, garantindo que a gramática esteja impecável e o tom seja sempre o mais profissional e coerente possível para clientes e parceiros.
+4. Estratégia e Mercado: 
+• Melhor Pós-Venda: A IA está ajudando a analisar o mercado para achar as melhores soluções e ideias para melhorar o nosso pós-venda. O objetivo é a satisfação e fidelização total do cliente!
+• Análise da Concorrência no Mapa: Estou usando ferramentas de análise geográfica e de texto para entender o que a concorrência está fazendo em cada estado do Brasil. 
+</t>
+  </si>
+  <si>
+    <t>Automatização de tarefa: Colaborador criou uma ferramenta que facilita o dia a dia do time de abastecimento. Ferramenta (EXCEL) em funcionamento com senha na rede para regra de abastecimento de filiais. Possível levantar os itens para romaneio. Identifica material em trânsito, analisa o que pode retornar ao CD.
+Cria 5 tabelas dinâmicas com itens zero, zero a um, diversas regras. Colaborador treinou a equipe.</t>
+  </si>
+  <si>
+    <t>Maria identificou uma oportunidade fiscal e estruturou uma metodologia replicável que transforma a conformidade tributária em geração de valor para a empresa.
+Diante de uma demanda da filial, rapidamente identificou o potencial estratégico do Crédito Outorgado de ICMS e transformou uma questão operacional em uma oportunidade de valor.
+Maria desenvolveu autonomamente:
+Estudo individual e aprofundado da legislação aplicável
+Metodologia própria para identificação e apuração
+Estratégia de integração com TI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Objetivo do Agente1: gerar análises objetivas e baseadas em dados sobre o desempenho individual de vendedores.
+• Diagnóstico preciso;
+• Desenvolvimento de planos de ação personalizados;
+• Estabelecimento de critérios objetivos de decisão;
+• Geração de relatórios.
+Objetivo do Agente2: desenvolver estratégias personalizadas e escaláveis para reativar clientes inativos.
+• Segmentação e categorização automática dos clientes inativos entre prospects e ex-clientes;
+• Análise do histórico de interações;
+• Definição exata da família de produtos mais adequada para cada perfil de cliente, considerando histórico, necessidades e aderência ao portfólio da empresa;
+• Desenvolvimento de estratégias de abordagem específicas por segmento;
+• Criação de scripts e roteiros detalhados de atendimento, prontos para uso pela equipe comercial, garantindo padronização, clareza e foco em reconversão;
+• Estabelecimento de métricas de sucesso (taxa de reativação, retomada de contato, reuniões agendadas, ticket reativado, tempo médio de reconversão) para monitorar e otimizar continuamente a eficácia das ações de reativação.
+Objetivo do Agente3: gerar relatórios estratégicos de prospecção que identifiquem novos clientes potenciais alinhados com as metas de vendas 
+• Integração com fontes abertas e bases públicas para pesquisa de empresas-alvo;
+• Coleta estruturada de dados;
+• Análise de potencial de conversão baseada em perfil financeiro, histórico do setor e alinhamento com os produtos;
+• Criação de estratégias personalizadas de abordagem, considerando necessidades do cliente e diferenciais;
+• Geração de relatórios estratégicos claros e objetivos;
+• Recomendações finais para maximizar conversão (ex.: priorização por porte, região ou histórico de compra).
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Em 2025, foi implantado a automatização de pagamento dos fretes homologados, integrando em nosso sistema SPR/SISPRO, através de uma API. A plataforma permitiu uma integração direta com o sistema, desde a classificação fiscal, conciliação contábil e pagamento, facilitando o monitoramento em tempo real das integrações e assegurando uma gestão mais eficiente dos pagamentos. Foram incorporados também mecanismos para o tratamento de exceções, ajustes e estornos, assegurando flexibilidade operacional e consistência dos dados. 
+O projeto foi um esforço conjunto entre as equipes de Financeiro, Logística, Tributário, Contabilidade e Tecnologia da Informação e até o final do ano de 2025 já tínhamos 14 transportadoras rodando nesse formato.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mateus Barreto </t>
+  </si>
+  <si>
+    <t>Colaborador atuou com processos de melhorias em: Organização do Fluxo de Cancelamentos; Regularização dos RMAs entre Transporte e Expedição; Controle e Redução do Volume de Chamados.</t>
+  </si>
+  <si>
+    <t>Matheus atuou na reestruturação da área de precificação, transformando um processo reativo e centralizado em um modelo de gestão ativo, descentralizado e baseado em dados.
+Ele padronizou processos operacionais, permitindo que as tarefas fossem distribuídas na equipe e reduzindo o risco operacional. As principais inovações foram solicitar ajustes no SPR para garantir melhor velocidade analítica e operacional e a implementação de IA para analisar os preços da concorrência, parametrizando as decisões, aumentando nossa competitividade. Além disso, está criando dashboards e atuando com a melhoria continua de sistemas, que permitem à equipe diminuir a análise manual e passar a fazer uma gestão em massa, mais ágil e estratégica.</t>
+  </si>
+  <si>
+    <t>Foi aprimorado o processo de coleta de óleo no setor CNC. Anteriormente, todo o óleo gerado pelas máquinas era descartado, sendo que esse descarte é pago. Com a implementação de recipientes específicos para a separação dessa coleta, reduziu-se o descarte de óleo que pode ser reutilizado, aumentando a vida útil do óleo que antes era inutilizado. Essa mudança resultou em menor volume de descarte pago e menor necessidade de reposição periódica de óleo nas máquinas.
+(Conforme melhoria implementada no Projeto de Ideias BIZA nº 88.)</t>
+  </si>
+  <si>
+    <t>Em 2025, com a ajuda da Coordenadora Fiscal, a colaboradora estruturou melhorias no processo de RMA, incluindo a criação de um campo no sistema para registrar pendências fiscais, a substituição da planilha manual da Qualidade por abertura de chamados e a inclusão de informações essenciais na tela de chamados (tipo da nota, chave de acesso, número da NF e aprovação do gestor). Também conduziu uma gestão ativa dos RMAs em aberto, monitorando pendências, cobrando regularizações aos setores responsáveis e escalonando casos sem retorno.</t>
+  </si>
+  <si>
+    <t>Criação do projeto “Gestão à Vista – Regionalização Comercial na Mineração”. Estão sendo estruturadas as rotinas comerciais (agendas, visitas, ações e funil) através de Lists, Planner, CRM, Excel e Power BI, trazendo padronização, visibilidade e suporte à tomada de decisão.
+A iniciativa busca evoluir em três fases — Operacional, Estratégica e Analítica — criando uma base sólida para gestão por indicadores, maior eficiência e futura aplicação de IA.</t>
+  </si>
+  <si>
+    <t>Mineração</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Em maio 2025, implantamos a liberação automática de pedidos à vista pela modalidade de pagamento via PIX QR CODE. Além de implantar uma nova modalidade de pagamento aos nossos clientes, criamos e desenvolvemos uma integração via API entre o banco e o nosso sistema, agilizando e facilitando a comunicação.
+Além disso, foi criada uma tela no SPR WEB visível tanto para o Financeiro quanto para o Comercial. Através dela, conseguimos gerir os pedidos gerados à vista e o status do pagamento via PIX, sendo possível ações e consultas de vendas nessa modalidade para casos que a integração sistêmica falhar por oscilação na internet ou sistema bancário fora do ar.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Desenvolvimento do relatório de devolução no Flow:  Esse relatório contempla as informações dos sistemas que usamos (Sispro e SPR). Concentrando as informações necessárias em um único lugar, obtivemos ganho de tempo e eficiência operacional.
+</t>
+  </si>
+  <si>
+    <t>Rodrigo Ribeiro  de Brito</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Indicou a automatização de e-mails com informações congeladas e a disponibilização de dados diretamente na tela do CRM do vendedor, garantindo maior agilidade e transparência. Além disso, vem estudando os motivos de não positivação, explorando pontos como estoques, fichas não abertas e estudos de concentração e padrão, com foco em identificar oportunidades de melhoria. Trabalha na padronização do conceito de positivação e na conexão com suprimentos e precificação, buscando evoluir processos e propor soluções. Embora ainda haja um caminho a percorrer, já avançamos significativamente com engajamento das áreas e melhoria na positivação do Atacado SP, consolidando uma base sólida para resultados cada vez mais expressivos. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Otimização do Processo de Consulta de OC para Cobrança da Carteira
+Com foco em assertividade e redução de retrabalho, identificou uma oportunidade para seguir com a cobrança de clientes com pagamento via depósito. Em parceria com a TI, foi melhorado relatório já existente para atender a demanda, consolidando automaticamente as principais informações necessárias para a cobrança.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Natália desenvolveu e implementou um método de segmentação clusterizada de clientes, combinando CNAE, potencial de mercado e IA, com foco em trazer um olhar externo de mercado sobre a carteira de clientes. Essa iniciativa não substitui o modelo de segmentação interno existente; ela o complementa com uma perspectiva externa, mais orientada ao posicionamento do cliente no mercado, fortalecendo a tomada de decisão comercial e estratégica.
+A solução proposta em 2025 propõe responder a pergunta: “Como o nosso cliente se posiciona dentro do mercado em que atua?”
+Aplicou técnicas de clusterização (agrupamento) com apoio de IA para:
+- Agrupar clientes e potenciais clientes com características similares de mercado (segmento, porte, abrangência nacional, papel na cadeia – indústria, primário, terceiro elo, etc.);
+- Destacar grandes players e contas estratégicas, buscando dar maior atenção a eles;
+- Criar uma classificação de potencial coerente com o mercado, e não somente com o histórico de compras com o GHT.
+Desenvolveu uma visão de “mapa de mercado”, em que:
+- Clientes atuais foram reposicionados segundo seu real peso no mercado, e não apenas pelo faturamento atual com a empresa;
+- Foram identificados clientes relevantes fora do radar, ou seja, empresas que atuam fortemente nos nossos segmentos-alvo, mas que ainda não tinham relacionamento estruturado com a companhia.
+Gerou relatórios e materiais estratégicos para o time de Vendas, como:
+- Perfis resumidos de clientes atuais com potencial de alavancagem;
+- Listas de prospects priorizados para prospecção ativa, classificados por segmento, porte, potencial e aderência portfólio GHT;
+- Diretrizes de abordagem por tipo de cliente, sugerindo temas, ganchos comerciais e soluções mais aderentes.
+Na prática, a solução transformou um conjunto disperso de dados em uma inteligência de mercado estruturada, capaz de orientar:
+- Onde estão os maiores potenciais de crescimento?
+- Quais clientes atuais merecem uma atuação mais estratégica?
+- Quais grandes empresas ainda não estão no nosso radar, mas deveriam estar?
+</t>
+  </si>
+  <si>
+    <t>André Pascoal Rodrigues</t>
+  </si>
+  <si>
+    <t>Colaborador desenvolveu uma estratégia de inteligência de mercado com EXCEL extraído pela TI, para identificar oportunidades para o GHT. 
+Houve muita consulta para máquinas novas, mas estávamos sem peças. Em 30 dias, já tínhamos 80 part numbers. É possível identificar também os principais concorrentes.
+Planejamento de estoque: objetivo diminuir os itens sem giro. Colaborador identificou que não temos peças para máquinas pequenas, o que contribui para novos estudos e investimentos, se necessário.</t>
   </si>
 </sst>
 </file>
@@ -152,7 +675,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -162,6 +685,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -178,12 +707,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -194,6 +726,21 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -229,10 +776,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:D9" totalsRowShown="0">
-  <autoFilter ref="A1:D9" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D9">
-    <sortCondition ref="C1:C9"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:D60" totalsRowShown="0">
+  <autoFilter ref="A1:D60" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D60">
+    <sortCondition ref="A1:A60"/>
   </sortState>
   <tableColumns count="4">
     <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Nome colaborador(a)_x000a_" dataDxfId="3"/>
@@ -541,18 +1088,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="47.109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="18.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="38.21875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="117.21875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="38.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="19.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="28.44140625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="153.88671875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -562,123 +1109,834 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>13</v>
+      <c r="C1" s="4" t="s">
+        <v>69</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:4" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="94.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="127.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+      <c r="A13" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+      <c r="A14" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="111" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A17" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="302.39999999999998" x14ac:dyDescent="0.3">
+      <c r="A18" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A20" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="50.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A23" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A24" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A25" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="159.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A27" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A28" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+      <c r="A29" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="73.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A31" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A32" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A33" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="112.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="259.2" x14ac:dyDescent="0.3">
+      <c r="A35" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="216" x14ac:dyDescent="0.3">
+      <c r="A36" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A37" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="52.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+      <c r="A39" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D39" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="4" t="s">
+    </row>
+    <row r="40" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A40" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="B40" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A41" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="374.4" x14ac:dyDescent="0.3">
+      <c r="A42" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A43" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A44" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A45" s="6" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
+      <c r="B45" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="360" x14ac:dyDescent="0.3">
+      <c r="A46" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A47" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B47" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="4" t="s">
+      <c r="C47" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A48" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="186.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B49" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C49" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="D49" s="10" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B50" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C50" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D50" s="10" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A51" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A52" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A53" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C53" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="100.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="55.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C55" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="60.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A57" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="316.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" s="2" t="s">
+      <c r="B58" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C58" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="D58" s="10" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A59" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C59" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A60" s="6" t="s">
         <v>20</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C60" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>